<commit_message>
fixed export inventory item, fixed issue report, aging report and restock report
</commit_message>
<xml_diff>
--- a/inventory_format.xlsx
+++ b/inventory_format.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView activeTab="5" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView activeTab="6" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId4"/>
@@ -13,6 +13,7 @@
     <sheet name="Group" sheetId="4" r:id="rId7"/>
     <sheet name="Location" sheetId="5" r:id="rId8"/>
     <sheet name="Warehouse" sheetId="6" r:id="rId9"/>
+    <sheet name="UOM" sheetId="7" r:id="rId10"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="303">
   <si>
     <t>Item Description</t>
   </si>
@@ -34,7 +35,7 @@
     <t>Subcat Prefix</t>
   </si>
   <si>
-    <t>Unit</t>
+    <t>UOM ID</t>
   </si>
   <si>
     <t>PN No</t>
@@ -55,10 +56,10 @@
     <t>Instructions:</t>
   </si>
   <si>
-    <t>Get Cat ID, Subcat CatID and Subcat Prefix in the reference sheet</t>
-  </si>
-  <si>
-    <t>Leave PN No. column blank if there's none, system will generate if empty</t>
+    <t>Get Cat ID, Subcat ID, Subcat Prefix, UOM ID, Rack ID, Group ID, WH ID and Location ID in the reference sheet</t>
+  </si>
+  <si>
+    <t>Leave PN No. column blank if there's none, system will generate pn no. if empty</t>
   </si>
   <si>
     <t>Cat/Subcat ID</t>
@@ -830,6 +831,105 @@
   </si>
   <si>
     <t>CV Access Area Bay 2</t>
+  </si>
+  <si>
+    <t>UOM Name</t>
+  </si>
+  <si>
+    <t>bag/s</t>
+  </si>
+  <si>
+    <t>bar/s</t>
+  </si>
+  <si>
+    <t>bot/s</t>
+  </si>
+  <si>
+    <t>box/s</t>
+  </si>
+  <si>
+    <t>can/s</t>
+  </si>
+  <si>
+    <t>cart/s</t>
+  </si>
+  <si>
+    <t>cont/s</t>
+  </si>
+  <si>
+    <t>cu.m</t>
+  </si>
+  <si>
+    <t>cyl/s</t>
+  </si>
+  <si>
+    <t>drum/s</t>
+  </si>
+  <si>
+    <t>feet</t>
+  </si>
+  <si>
+    <t>gal/s</t>
+  </si>
+  <si>
+    <t>kg/s</t>
+  </si>
+  <si>
+    <t>lgth/s</t>
+  </si>
+  <si>
+    <t>ltr/s</t>
+  </si>
+  <si>
+    <t>mtr/s</t>
+  </si>
+  <si>
+    <t>pack/s</t>
+  </si>
+  <si>
+    <t>pad/s</t>
+  </si>
+  <si>
+    <t>pail/s</t>
+  </si>
+  <si>
+    <t>pair/s</t>
+  </si>
+  <si>
+    <t>pc/s</t>
+  </si>
+  <si>
+    <t>ream/s</t>
+  </si>
+  <si>
+    <t>roll/s</t>
+  </si>
+  <si>
+    <t>sack/s</t>
+  </si>
+  <si>
+    <t>set/s</t>
+  </si>
+  <si>
+    <t>sht/s</t>
+  </si>
+  <si>
+    <t>tab/s</t>
+  </si>
+  <si>
+    <t>tube/s</t>
+  </si>
+  <si>
+    <t>unit/s</t>
+  </si>
+  <si>
+    <t>grm/s</t>
+  </si>
+  <si>
+    <t>assy/s</t>
+  </si>
+  <si>
+    <t>lot/s</t>
   </si>
 </sst>
 </file>
@@ -3191,6 +3291,75 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
+    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>269</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <printOptions gridLines="false" gridLinesSet="true"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
+  <dimension ref="A1:B33"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
@@ -3199,10 +3368,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>264</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>265</v>
+        <v>270</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -3210,7 +3379,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -3218,7 +3387,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -3226,7 +3395,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>268</v>
+        <v>273</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -3234,7 +3403,231 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>269</v>
+        <v>274</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>302</v>
       </c>
     </row>
   </sheetData>

</xml_diff>